<commit_message>
*Finished Validation Results documentation* *Changes test case names*
</commit_message>
<xml_diff>
--- a/Documentation/Test_Cases_Functionality.xlsx
+++ b/Documentation/Test_Cases_Functionality.xlsx
@@ -5,56 +5,56 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Users\Jakob\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakob\Documents\PharmaCare\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B5BF0CE0-677E-42E2-9CEB-E093FB916756}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BE3A4C20-DC75-49B2-9915-ED6304D81C7C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14610" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCaseList" sheetId="2" r:id="rId1"/>
-    <sheet name="TestReport" sheetId="8" r:id="rId2"/>
-    <sheet name="Rework1" sheetId="6" r:id="rId3"/>
-    <sheet name="Rework2" sheetId="7" r:id="rId4"/>
+    <sheet name="Test Case 1" sheetId="8" r:id="rId2"/>
+    <sheet name="Test Case 2" sheetId="6" r:id="rId3"/>
+    <sheet name="Test Case 3" sheetId="7" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="ABS" localSheetId="1">#REF!</definedName>
     <definedName name="ABS" localSheetId="3">#REF!</definedName>
-    <definedName name="ABS" localSheetId="1">#REF!</definedName>
     <definedName name="ABS">#REF!</definedName>
-    <definedName name="CRITICALITY" localSheetId="2">Rework1!$A$72:$A$76</definedName>
-    <definedName name="CRITICALITY" localSheetId="3">Rework2!$A$72:$A$76</definedName>
-    <definedName name="CRITICALITY" localSheetId="1">TestReport!$A$86:$A$90</definedName>
+    <definedName name="CRITICALITY" localSheetId="1">'Test Case 1'!$A$86:$A$90</definedName>
+    <definedName name="CRITICALITY" localSheetId="2">'Test Case 2'!$A$72:$A$76</definedName>
+    <definedName name="CRITICALITY" localSheetId="3">'Test Case 3'!$A$72:$A$76</definedName>
     <definedName name="CRITICALITY">#REF!</definedName>
-    <definedName name="no" localSheetId="2">Rework1!#REF!</definedName>
-    <definedName name="no" localSheetId="3">Rework2!#REF!</definedName>
-    <definedName name="no" localSheetId="1">TestReport!#REF!</definedName>
+    <definedName name="no" localSheetId="1">'Test Case 1'!#REF!</definedName>
+    <definedName name="no" localSheetId="2">'Test Case 2'!#REF!</definedName>
+    <definedName name="no" localSheetId="3">'Test Case 3'!#REF!</definedName>
     <definedName name="no">#REF!</definedName>
-    <definedName name="nono" localSheetId="2">Rework1!$E$72:$E$73</definedName>
-    <definedName name="nono" localSheetId="3">Rework2!$E$72:$E$73</definedName>
-    <definedName name="nono" localSheetId="1">TestReport!$E$64:$E$65</definedName>
+    <definedName name="nono" localSheetId="1">'Test Case 1'!$E$64:$E$65</definedName>
+    <definedName name="nono" localSheetId="2">'Test Case 2'!$E$72:$E$73</definedName>
+    <definedName name="nono" localSheetId="3">'Test Case 3'!$E$72:$E$73</definedName>
     <definedName name="nono">#REF!</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="2">Rework1!$8:$8</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="3">Rework2!$8:$8</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="1">TestReport!$8:$8</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">'Test Case 1'!$8:$8</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="2">'Test Case 2'!$8:$8</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="3">'Test Case 3'!$8:$8</definedName>
+    <definedName name="SAM" localSheetId="1">#REF!</definedName>
     <definedName name="SAM" localSheetId="3">#REF!</definedName>
-    <definedName name="SAM" localSheetId="1">#REF!</definedName>
     <definedName name="SAM">#REF!</definedName>
-    <definedName name="testing" localSheetId="2">Rework1!$F$72:$F$81</definedName>
-    <definedName name="testing" localSheetId="3">Rework2!$F$72:$F$81</definedName>
-    <definedName name="testing" localSheetId="1">TestReport!$F$64:$F$73</definedName>
+    <definedName name="testing" localSheetId="1">'Test Case 1'!$F$64:$F$73</definedName>
+    <definedName name="testing" localSheetId="2">'Test Case 2'!$F$72:$F$81</definedName>
+    <definedName name="testing" localSheetId="3">'Test Case 3'!$F$72:$F$81</definedName>
     <definedName name="testing">#REF!</definedName>
-    <definedName name="yes" localSheetId="2">Rework1!#REF!</definedName>
-    <definedName name="yes" localSheetId="3">Rework2!#REF!</definedName>
-    <definedName name="yes" localSheetId="1">TestReport!#REF!</definedName>
+    <definedName name="yes" localSheetId="1">'Test Case 1'!#REF!</definedName>
+    <definedName name="yes" localSheetId="2">'Test Case 2'!#REF!</definedName>
+    <definedName name="yes" localSheetId="3">'Test Case 3'!#REF!</definedName>
     <definedName name="yes">#REF!</definedName>
-    <definedName name="yes1" localSheetId="2">Rework1!#REF!</definedName>
-    <definedName name="yes1" localSheetId="3">Rework2!#REF!</definedName>
-    <definedName name="yes1" localSheetId="1">TestReport!#REF!</definedName>
+    <definedName name="yes1" localSheetId="1">'Test Case 1'!#REF!</definedName>
+    <definedName name="yes1" localSheetId="2">'Test Case 2'!#REF!</definedName>
+    <definedName name="yes1" localSheetId="3">'Test Case 3'!#REF!</definedName>
     <definedName name="yes1">#REF!</definedName>
-    <definedName name="yes2" localSheetId="2">Rework1!$C$72:$C$73</definedName>
-    <definedName name="yes2" localSheetId="3">Rework2!$C$72:$C$73</definedName>
-    <definedName name="yes2" localSheetId="1">TestReport!$C$64:$C$65</definedName>
+    <definedName name="yes2" localSheetId="1">'Test Case 1'!$C$64:$C$65</definedName>
+    <definedName name="yes2" localSheetId="2">'Test Case 2'!$C$72:$C$73</definedName>
+    <definedName name="yes2" localSheetId="3">'Test Case 3'!$C$72:$C$73</definedName>
     <definedName name="yes2">#REF!</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
@@ -1745,49 +1745,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="28" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1829,6 +1790,54 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="28" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1837,15 +1846,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4182,7 +4182,7 @@
   <dimension ref="A1:L95"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4200,112 +4200,112 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="68.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="85" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="70"/>
+      <c r="B1" s="86"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
+      <c r="I1" s="87"/>
+      <c r="J1" s="87"/>
+      <c r="K1" s="88"/>
     </row>
     <row r="2" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="72"/>
-      <c r="C2" s="73">
+      <c r="B2" s="68"/>
+      <c r="C2" s="89">
         <v>43438</v>
       </c>
-      <c r="D2" s="73"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="74"/>
-      <c r="J2" s="75" t="s">
+      <c r="D2" s="89"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="91" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="77">
+      <c r="K2" s="93">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="71" t="s">
+      <c r="A3" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="72"/>
-      <c r="C3" s="79" t="s">
+      <c r="B3" s="68"/>
+      <c r="C3" s="95" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="76"/>
-      <c r="K3" s="78"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="92"/>
+      <c r="K3" s="94"/>
     </row>
     <row r="4" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="82"/>
-      <c r="D4" s="82"/>
-      <c r="E4" s="82"/>
-      <c r="F4" s="82"/>
-      <c r="G4" s="82"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="82"/>
-      <c r="J4" s="82"/>
-      <c r="K4" s="83"/>
+      <c r="B4" s="68"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="69"/>
+      <c r="I4" s="69"/>
+      <c r="J4" s="69"/>
+      <c r="K4" s="70"/>
     </row>
     <row r="5" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="71" t="s">
+      <c r="A5" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="72"/>
-      <c r="C5" s="98" t="s">
+      <c r="B5" s="68"/>
+      <c r="C5" s="82" t="s">
         <v>163</v>
       </c>
-      <c r="D5" s="99"/>
-      <c r="E5" s="99"/>
-      <c r="F5" s="99"/>
-      <c r="G5" s="99"/>
-      <c r="H5" s="99"/>
-      <c r="I5" s="99"/>
-      <c r="J5" s="99"/>
-      <c r="K5" s="100"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
+      <c r="H5" s="83"/>
+      <c r="I5" s="83"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="84"/>
     </row>
     <row r="6" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="71" t="s">
+      <c r="A6" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="72"/>
-      <c r="C6" s="82" t="s">
+      <c r="B6" s="68"/>
+      <c r="C6" s="69" t="s">
         <v>166</v>
       </c>
-      <c r="D6" s="82"/>
-      <c r="E6" s="82"/>
-      <c r="F6" s="82"/>
-      <c r="G6" s="82"/>
-      <c r="H6" s="82"/>
-      <c r="I6" s="82"/>
-      <c r="J6" s="82"/>
-      <c r="K6" s="83"/>
+      <c r="D6" s="69"/>
+      <c r="E6" s="69"/>
+      <c r="F6" s="69"/>
+      <c r="G6" s="69"/>
+      <c r="H6" s="69"/>
+      <c r="I6" s="69"/>
+      <c r="J6" s="69"/>
+      <c r="K6" s="70"/>
     </row>
     <row r="7" spans="1:12" ht="96" x14ac:dyDescent="0.25">
-      <c r="A7" s="84" t="s">
+      <c r="A7" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="85"/>
+      <c r="B7" s="72"/>
       <c r="C7" s="1" t="s">
         <v>27</v>
       </c>
@@ -5582,17 +5582,17 @@
       <c r="B56" s="50"/>
       <c r="C56" s="51"/>
       <c r="D56" s="48"/>
-      <c r="E56" s="86" t="s">
+      <c r="E56" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="F56" s="87"/>
-      <c r="G56" s="87"/>
-      <c r="H56" s="87"/>
-      <c r="I56" s="88"/>
-      <c r="J56" s="89" t="s">
+      <c r="F56" s="74"/>
+      <c r="G56" s="74"/>
+      <c r="H56" s="74"/>
+      <c r="I56" s="75"/>
+      <c r="J56" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="K56" s="93"/>
+      <c r="K56" s="80"/>
     </row>
     <row r="57" spans="1:11" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="27">
@@ -5601,13 +5601,13 @@
       <c r="B57" s="50"/>
       <c r="C57" s="51"/>
       <c r="D57" s="48"/>
-      <c r="E57" s="89"/>
-      <c r="F57" s="87"/>
-      <c r="G57" s="87"/>
-      <c r="H57" s="87"/>
-      <c r="I57" s="88"/>
-      <c r="J57" s="89"/>
-      <c r="K57" s="93"/>
+      <c r="E57" s="76"/>
+      <c r="F57" s="74"/>
+      <c r="G57" s="74"/>
+      <c r="H57" s="74"/>
+      <c r="I57" s="75"/>
+      <c r="J57" s="76"/>
+      <c r="K57" s="80"/>
     </row>
     <row r="58" spans="1:11" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="27">
@@ -5616,13 +5616,13 @@
       <c r="B58" s="50"/>
       <c r="C58" s="51"/>
       <c r="D58" s="48"/>
-      <c r="E58" s="89"/>
-      <c r="F58" s="87"/>
-      <c r="G58" s="87"/>
-      <c r="H58" s="87"/>
-      <c r="I58" s="88"/>
-      <c r="J58" s="89"/>
-      <c r="K58" s="93"/>
+      <c r="E58" s="76"/>
+      <c r="F58" s="74"/>
+      <c r="G58" s="74"/>
+      <c r="H58" s="74"/>
+      <c r="I58" s="75"/>
+      <c r="J58" s="76"/>
+      <c r="K58" s="80"/>
     </row>
     <row r="59" spans="1:11" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="27">
@@ -5631,13 +5631,13 @@
       <c r="B59" s="50"/>
       <c r="C59" s="51"/>
       <c r="D59" s="48"/>
-      <c r="E59" s="89"/>
-      <c r="F59" s="87"/>
-      <c r="G59" s="87"/>
-      <c r="H59" s="87"/>
-      <c r="I59" s="88"/>
-      <c r="J59" s="89"/>
-      <c r="K59" s="93"/>
+      <c r="E59" s="76"/>
+      <c r="F59" s="74"/>
+      <c r="G59" s="74"/>
+      <c r="H59" s="74"/>
+      <c r="I59" s="75"/>
+      <c r="J59" s="76"/>
+      <c r="K59" s="80"/>
     </row>
     <row r="60" spans="1:11" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="27">
@@ -5646,13 +5646,13 @@
       <c r="B60" s="50"/>
       <c r="C60" s="51"/>
       <c r="D60" s="48"/>
-      <c r="E60" s="89"/>
-      <c r="F60" s="87"/>
-      <c r="G60" s="87"/>
-      <c r="H60" s="87"/>
-      <c r="I60" s="88"/>
-      <c r="J60" s="89"/>
-      <c r="K60" s="93"/>
+      <c r="E60" s="76"/>
+      <c r="F60" s="74"/>
+      <c r="G60" s="74"/>
+      <c r="H60" s="74"/>
+      <c r="I60" s="75"/>
+      <c r="J60" s="76"/>
+      <c r="K60" s="80"/>
     </row>
     <row r="61" spans="1:11" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="27">
@@ -5661,13 +5661,13 @@
       <c r="B61" s="50"/>
       <c r="C61" s="51"/>
       <c r="D61" s="48"/>
-      <c r="E61" s="89"/>
-      <c r="F61" s="87"/>
-      <c r="G61" s="87"/>
-      <c r="H61" s="87"/>
-      <c r="I61" s="88"/>
-      <c r="J61" s="89"/>
-      <c r="K61" s="93"/>
+      <c r="E61" s="76"/>
+      <c r="F61" s="74"/>
+      <c r="G61" s="74"/>
+      <c r="H61" s="74"/>
+      <c r="I61" s="75"/>
+      <c r="J61" s="76"/>
+      <c r="K61" s="80"/>
     </row>
     <row r="62" spans="1:11" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="27">
@@ -5676,13 +5676,13 @@
       <c r="B62" s="50"/>
       <c r="C62" s="51"/>
       <c r="D62" s="48"/>
-      <c r="E62" s="89"/>
-      <c r="F62" s="87"/>
-      <c r="G62" s="87"/>
-      <c r="H62" s="87"/>
-      <c r="I62" s="88"/>
-      <c r="J62" s="89"/>
-      <c r="K62" s="93"/>
+      <c r="E62" s="76"/>
+      <c r="F62" s="74"/>
+      <c r="G62" s="74"/>
+      <c r="H62" s="74"/>
+      <c r="I62" s="75"/>
+      <c r="J62" s="76"/>
+      <c r="K62" s="80"/>
     </row>
     <row r="63" spans="1:11" ht="26.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="27">
@@ -5691,13 +5691,13 @@
       <c r="B63" s="52"/>
       <c r="C63" s="53"/>
       <c r="D63" s="49"/>
-      <c r="E63" s="90"/>
-      <c r="F63" s="91"/>
-      <c r="G63" s="91"/>
-      <c r="H63" s="91"/>
-      <c r="I63" s="92"/>
-      <c r="J63" s="90"/>
-      <c r="K63" s="94"/>
+      <c r="E63" s="77"/>
+      <c r="F63" s="78"/>
+      <c r="G63" s="78"/>
+      <c r="H63" s="78"/>
+      <c r="I63" s="79"/>
+      <c r="J63" s="77"/>
+      <c r="K63" s="81"/>
     </row>
     <row r="64" spans="1:11" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="27">
@@ -5949,11 +5949,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:K6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="E56:I63"/>
-    <mergeCell ref="J56:K63"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:K4"/>
     <mergeCell ref="A5:B5"/>
@@ -5965,6 +5960,11 @@
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:I3"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:K6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="E56:I63"/>
+    <mergeCell ref="J56:K63"/>
   </mergeCells>
   <conditionalFormatting sqref="I49:I55">
     <cfRule type="cellIs" dxfId="231" priority="107" operator="equal">
@@ -6282,7 +6282,7 @@
   </sheetPr>
   <dimension ref="A1:L81"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A6" sqref="A6:K6"/>
     </sheetView>
   </sheetViews>
@@ -6301,112 +6301,112 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="68.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="85" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="70"/>
+      <c r="B1" s="86"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
+      <c r="I1" s="87"/>
+      <c r="J1" s="87"/>
+      <c r="K1" s="88"/>
     </row>
     <row r="2" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="72"/>
-      <c r="C2" s="73">
+      <c r="B2" s="68"/>
+      <c r="C2" s="89">
         <v>43438</v>
       </c>
-      <c r="D2" s="73"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="74"/>
-      <c r="J2" s="75" t="s">
+      <c r="D2" s="89"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="91" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="77">
+      <c r="K2" s="93">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="71" t="s">
+      <c r="A3" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="72"/>
-      <c r="C3" s="79" t="s">
+      <c r="B3" s="68"/>
+      <c r="C3" s="95" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="76"/>
-      <c r="K3" s="78"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="92"/>
+      <c r="K3" s="94"/>
     </row>
     <row r="4" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="82"/>
-      <c r="D4" s="82"/>
-      <c r="E4" s="82"/>
-      <c r="F4" s="82"/>
-      <c r="G4" s="82"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="82"/>
-      <c r="J4" s="82"/>
-      <c r="K4" s="83"/>
+      <c r="B4" s="68"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="69"/>
+      <c r="I4" s="69"/>
+      <c r="J4" s="69"/>
+      <c r="K4" s="70"/>
     </row>
     <row r="5" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="71" t="s">
+      <c r="A5" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="72"/>
-      <c r="C5" s="98" t="s">
+      <c r="B5" s="68"/>
+      <c r="C5" s="82" t="s">
         <v>163</v>
       </c>
-      <c r="D5" s="99"/>
-      <c r="E5" s="99"/>
-      <c r="F5" s="99"/>
-      <c r="G5" s="99"/>
-      <c r="H5" s="99"/>
-      <c r="I5" s="99"/>
-      <c r="J5" s="99"/>
-      <c r="K5" s="100"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
+      <c r="H5" s="83"/>
+      <c r="I5" s="83"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="84"/>
     </row>
     <row r="6" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="71" t="s">
+      <c r="A6" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="72"/>
-      <c r="C6" s="82" t="s">
+      <c r="B6" s="68"/>
+      <c r="C6" s="69" t="s">
         <v>165</v>
       </c>
-      <c r="D6" s="82"/>
-      <c r="E6" s="82"/>
-      <c r="F6" s="82"/>
-      <c r="G6" s="82"/>
-      <c r="H6" s="82"/>
-      <c r="I6" s="82"/>
-      <c r="J6" s="82"/>
-      <c r="K6" s="83"/>
+      <c r="D6" s="69"/>
+      <c r="E6" s="69"/>
+      <c r="F6" s="69"/>
+      <c r="G6" s="69"/>
+      <c r="H6" s="69"/>
+      <c r="I6" s="69"/>
+      <c r="J6" s="69"/>
+      <c r="K6" s="70"/>
     </row>
     <row r="7" spans="1:12" ht="96" x14ac:dyDescent="0.25">
-      <c r="A7" s="84" t="s">
+      <c r="A7" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="95"/>
+      <c r="B7" s="98"/>
       <c r="C7" s="1" t="s">
         <v>27</v>
       </c>
@@ -7883,114 +7883,114 @@
       </c>
     </row>
     <row r="64" spans="1:11" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="96" t="s">
+      <c r="A64" s="99" t="s">
         <v>34</v>
       </c>
-      <c r="B64" s="87"/>
-      <c r="C64" s="88"/>
+      <c r="B64" s="74"/>
+      <c r="C64" s="75"/>
       <c r="D64" s="45"/>
-      <c r="E64" s="86" t="s">
+      <c r="E64" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="F64" s="87"/>
-      <c r="G64" s="87"/>
-      <c r="H64" s="87"/>
-      <c r="I64" s="88"/>
-      <c r="J64" s="89" t="s">
+      <c r="F64" s="74"/>
+      <c r="G64" s="74"/>
+      <c r="H64" s="74"/>
+      <c r="I64" s="75"/>
+      <c r="J64" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="K64" s="93"/>
+      <c r="K64" s="80"/>
     </row>
     <row r="65" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="96"/>
-      <c r="B65" s="87"/>
-      <c r="C65" s="88"/>
+      <c r="A65" s="99"/>
+      <c r="B65" s="74"/>
+      <c r="C65" s="75"/>
       <c r="D65" s="45"/>
-      <c r="E65" s="89"/>
-      <c r="F65" s="87"/>
-      <c r="G65" s="87"/>
-      <c r="H65" s="87"/>
-      <c r="I65" s="88"/>
-      <c r="J65" s="89"/>
-      <c r="K65" s="93"/>
+      <c r="E65" s="76"/>
+      <c r="F65" s="74"/>
+      <c r="G65" s="74"/>
+      <c r="H65" s="74"/>
+      <c r="I65" s="75"/>
+      <c r="J65" s="76"/>
+      <c r="K65" s="80"/>
     </row>
     <row r="66" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="96"/>
-      <c r="B66" s="87"/>
-      <c r="C66" s="88"/>
+      <c r="A66" s="99"/>
+      <c r="B66" s="74"/>
+      <c r="C66" s="75"/>
       <c r="D66" s="45"/>
-      <c r="E66" s="89"/>
-      <c r="F66" s="87"/>
-      <c r="G66" s="87"/>
-      <c r="H66" s="87"/>
-      <c r="I66" s="88"/>
-      <c r="J66" s="89"/>
-      <c r="K66" s="93"/>
+      <c r="E66" s="76"/>
+      <c r="F66" s="74"/>
+      <c r="G66" s="74"/>
+      <c r="H66" s="74"/>
+      <c r="I66" s="75"/>
+      <c r="J66" s="76"/>
+      <c r="K66" s="80"/>
     </row>
     <row r="67" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="96"/>
-      <c r="B67" s="87"/>
-      <c r="C67" s="88"/>
+      <c r="A67" s="99"/>
+      <c r="B67" s="74"/>
+      <c r="C67" s="75"/>
       <c r="D67" s="45"/>
-      <c r="E67" s="89"/>
-      <c r="F67" s="87"/>
-      <c r="G67" s="87"/>
-      <c r="H67" s="87"/>
-      <c r="I67" s="88"/>
-      <c r="J67" s="89"/>
-      <c r="K67" s="93"/>
+      <c r="E67" s="76"/>
+      <c r="F67" s="74"/>
+      <c r="G67" s="74"/>
+      <c r="H67" s="74"/>
+      <c r="I67" s="75"/>
+      <c r="J67" s="76"/>
+      <c r="K67" s="80"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A68" s="96"/>
-      <c r="B68" s="87"/>
-      <c r="C68" s="88"/>
+      <c r="A68" s="99"/>
+      <c r="B68" s="74"/>
+      <c r="C68" s="75"/>
       <c r="D68" s="45"/>
-      <c r="E68" s="89"/>
-      <c r="F68" s="87"/>
-      <c r="G68" s="87"/>
-      <c r="H68" s="87"/>
-      <c r="I68" s="88"/>
-      <c r="J68" s="89"/>
-      <c r="K68" s="93"/>
+      <c r="E68" s="76"/>
+      <c r="F68" s="74"/>
+      <c r="G68" s="74"/>
+      <c r="H68" s="74"/>
+      <c r="I68" s="75"/>
+      <c r="J68" s="76"/>
+      <c r="K68" s="80"/>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A69" s="96"/>
-      <c r="B69" s="87"/>
-      <c r="C69" s="88"/>
+      <c r="A69" s="99"/>
+      <c r="B69" s="74"/>
+      <c r="C69" s="75"/>
       <c r="D69" s="45"/>
-      <c r="E69" s="89"/>
-      <c r="F69" s="87"/>
-      <c r="G69" s="87"/>
-      <c r="H69" s="87"/>
-      <c r="I69" s="88"/>
-      <c r="J69" s="89"/>
-      <c r="K69" s="93"/>
+      <c r="E69" s="76"/>
+      <c r="F69" s="74"/>
+      <c r="G69" s="74"/>
+      <c r="H69" s="74"/>
+      <c r="I69" s="75"/>
+      <c r="J69" s="76"/>
+      <c r="K69" s="80"/>
     </row>
     <row r="70" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="96"/>
-      <c r="B70" s="87"/>
-      <c r="C70" s="88"/>
+      <c r="A70" s="99"/>
+      <c r="B70" s="74"/>
+      <c r="C70" s="75"/>
       <c r="D70" s="45"/>
-      <c r="E70" s="89"/>
-      <c r="F70" s="87"/>
-      <c r="G70" s="87"/>
-      <c r="H70" s="87"/>
-      <c r="I70" s="88"/>
-      <c r="J70" s="89"/>
-      <c r="K70" s="93"/>
+      <c r="E70" s="76"/>
+      <c r="F70" s="74"/>
+      <c r="G70" s="74"/>
+      <c r="H70" s="74"/>
+      <c r="I70" s="75"/>
+      <c r="J70" s="76"/>
+      <c r="K70" s="80"/>
     </row>
     <row r="71" spans="1:11" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="97"/>
-      <c r="B71" s="91"/>
-      <c r="C71" s="92"/>
+      <c r="A71" s="100"/>
+      <c r="B71" s="78"/>
+      <c r="C71" s="79"/>
       <c r="D71" s="46"/>
-      <c r="E71" s="90"/>
-      <c r="F71" s="91"/>
-      <c r="G71" s="91"/>
-      <c r="H71" s="91"/>
-      <c r="I71" s="92"/>
-      <c r="J71" s="90"/>
-      <c r="K71" s="94"/>
+      <c r="E71" s="77"/>
+      <c r="F71" s="78"/>
+      <c r="G71" s="78"/>
+      <c r="H71" s="78"/>
+      <c r="I71" s="79"/>
+      <c r="J71" s="77"/>
+      <c r="K71" s="81"/>
     </row>
     <row r="72" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="28" t="s">
@@ -8156,12 +8156,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:K6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A64:C71"/>
-    <mergeCell ref="E64:I71"/>
-    <mergeCell ref="J64:K71"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:K4"/>
     <mergeCell ref="A5:B5"/>
@@ -8173,6 +8167,12 @@
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:I3"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:K6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A64:C71"/>
+    <mergeCell ref="E64:I71"/>
+    <mergeCell ref="J64:K71"/>
   </mergeCells>
   <conditionalFormatting sqref="I49:I63">
     <cfRule type="cellIs" dxfId="159" priority="73" operator="equal">
@@ -8541,112 +8541,112 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="68.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="85" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="70"/>
+      <c r="B1" s="86"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
+      <c r="I1" s="87"/>
+      <c r="J1" s="87"/>
+      <c r="K1" s="88"/>
     </row>
     <row r="2" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="72"/>
-      <c r="C2" s="73">
+      <c r="B2" s="68"/>
+      <c r="C2" s="89">
         <v>43438</v>
       </c>
-      <c r="D2" s="73"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="74"/>
-      <c r="J2" s="75" t="s">
+      <c r="D2" s="89"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="91" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="77">
+      <c r="K2" s="93">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="71" t="s">
+      <c r="A3" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="72"/>
-      <c r="C3" s="79" t="s">
+      <c r="B3" s="68"/>
+      <c r="C3" s="95" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="76"/>
-      <c r="K3" s="78"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="92"/>
+      <c r="K3" s="94"/>
     </row>
     <row r="4" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="98"/>
-      <c r="D4" s="99"/>
-      <c r="E4" s="99"/>
-      <c r="F4" s="99"/>
-      <c r="G4" s="99"/>
-      <c r="H4" s="99"/>
-      <c r="I4" s="99"/>
-      <c r="J4" s="99"/>
-      <c r="K4" s="100"/>
+      <c r="B4" s="68"/>
+      <c r="C4" s="82"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="83"/>
+      <c r="J4" s="83"/>
+      <c r="K4" s="84"/>
     </row>
     <row r="5" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="71" t="s">
+      <c r="A5" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="72"/>
-      <c r="C5" s="98" t="s">
+      <c r="B5" s="68"/>
+      <c r="C5" s="82" t="s">
         <v>163</v>
       </c>
-      <c r="D5" s="99"/>
-      <c r="E5" s="99"/>
-      <c r="F5" s="99"/>
-      <c r="G5" s="99"/>
-      <c r="H5" s="99"/>
-      <c r="I5" s="99"/>
-      <c r="J5" s="99"/>
-      <c r="K5" s="100"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
+      <c r="H5" s="83"/>
+      <c r="I5" s="83"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="84"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="71" t="s">
+      <c r="A6" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="72"/>
-      <c r="C6" s="98" t="s">
+      <c r="B6" s="68"/>
+      <c r="C6" s="82" t="s">
         <v>164</v>
       </c>
-      <c r="D6" s="99"/>
-      <c r="E6" s="99"/>
-      <c r="F6" s="99"/>
-      <c r="G6" s="99"/>
-      <c r="H6" s="99"/>
-      <c r="I6" s="99"/>
-      <c r="J6" s="99"/>
-      <c r="K6" s="100"/>
+      <c r="D6" s="83"/>
+      <c r="E6" s="83"/>
+      <c r="F6" s="83"/>
+      <c r="G6" s="83"/>
+      <c r="H6" s="83"/>
+      <c r="I6" s="83"/>
+      <c r="J6" s="83"/>
+      <c r="K6" s="84"/>
     </row>
     <row r="7" spans="1:12" ht="96" x14ac:dyDescent="0.25">
-      <c r="A7" s="84" t="s">
+      <c r="A7" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="95"/>
+      <c r="B7" s="98"/>
       <c r="C7" s="1" t="s">
         <v>27</v>
       </c>
@@ -10123,114 +10123,114 @@
       </c>
     </row>
     <row r="64" spans="1:11" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="96" t="s">
+      <c r="A64" s="99" t="s">
         <v>34</v>
       </c>
-      <c r="B64" s="87"/>
-      <c r="C64" s="88"/>
+      <c r="B64" s="74"/>
+      <c r="C64" s="75"/>
       <c r="D64" s="48"/>
-      <c r="E64" s="86" t="s">
+      <c r="E64" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="F64" s="87"/>
-      <c r="G64" s="87"/>
-      <c r="H64" s="87"/>
-      <c r="I64" s="88"/>
-      <c r="J64" s="89" t="s">
+      <c r="F64" s="74"/>
+      <c r="G64" s="74"/>
+      <c r="H64" s="74"/>
+      <c r="I64" s="75"/>
+      <c r="J64" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="K64" s="93"/>
+      <c r="K64" s="80"/>
     </row>
     <row r="65" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="96"/>
-      <c r="B65" s="87"/>
-      <c r="C65" s="88"/>
+      <c r="A65" s="99"/>
+      <c r="B65" s="74"/>
+      <c r="C65" s="75"/>
       <c r="D65" s="48"/>
-      <c r="E65" s="89"/>
-      <c r="F65" s="87"/>
-      <c r="G65" s="87"/>
-      <c r="H65" s="87"/>
-      <c r="I65" s="88"/>
-      <c r="J65" s="89"/>
-      <c r="K65" s="93"/>
+      <c r="E65" s="76"/>
+      <c r="F65" s="74"/>
+      <c r="G65" s="74"/>
+      <c r="H65" s="74"/>
+      <c r="I65" s="75"/>
+      <c r="J65" s="76"/>
+      <c r="K65" s="80"/>
     </row>
     <row r="66" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="96"/>
-      <c r="B66" s="87"/>
-      <c r="C66" s="88"/>
+      <c r="A66" s="99"/>
+      <c r="B66" s="74"/>
+      <c r="C66" s="75"/>
       <c r="D66" s="48"/>
-      <c r="E66" s="89"/>
-      <c r="F66" s="87"/>
-      <c r="G66" s="87"/>
-      <c r="H66" s="87"/>
-      <c r="I66" s="88"/>
-      <c r="J66" s="89"/>
-      <c r="K66" s="93"/>
+      <c r="E66" s="76"/>
+      <c r="F66" s="74"/>
+      <c r="G66" s="74"/>
+      <c r="H66" s="74"/>
+      <c r="I66" s="75"/>
+      <c r="J66" s="76"/>
+      <c r="K66" s="80"/>
     </row>
     <row r="67" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="96"/>
-      <c r="B67" s="87"/>
-      <c r="C67" s="88"/>
+      <c r="A67" s="99"/>
+      <c r="B67" s="74"/>
+      <c r="C67" s="75"/>
       <c r="D67" s="48"/>
-      <c r="E67" s="89"/>
-      <c r="F67" s="87"/>
-      <c r="G67" s="87"/>
-      <c r="H67" s="87"/>
-      <c r="I67" s="88"/>
-      <c r="J67" s="89"/>
-      <c r="K67" s="93"/>
+      <c r="E67" s="76"/>
+      <c r="F67" s="74"/>
+      <c r="G67" s="74"/>
+      <c r="H67" s="74"/>
+      <c r="I67" s="75"/>
+      <c r="J67" s="76"/>
+      <c r="K67" s="80"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A68" s="96"/>
-      <c r="B68" s="87"/>
-      <c r="C68" s="88"/>
+      <c r="A68" s="99"/>
+      <c r="B68" s="74"/>
+      <c r="C68" s="75"/>
       <c r="D68" s="48"/>
-      <c r="E68" s="89"/>
-      <c r="F68" s="87"/>
-      <c r="G68" s="87"/>
-      <c r="H68" s="87"/>
-      <c r="I68" s="88"/>
-      <c r="J68" s="89"/>
-      <c r="K68" s="93"/>
+      <c r="E68" s="76"/>
+      <c r="F68" s="74"/>
+      <c r="G68" s="74"/>
+      <c r="H68" s="74"/>
+      <c r="I68" s="75"/>
+      <c r="J68" s="76"/>
+      <c r="K68" s="80"/>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A69" s="96"/>
-      <c r="B69" s="87"/>
-      <c r="C69" s="88"/>
+      <c r="A69" s="99"/>
+      <c r="B69" s="74"/>
+      <c r="C69" s="75"/>
       <c r="D69" s="48"/>
-      <c r="E69" s="89"/>
-      <c r="F69" s="87"/>
-      <c r="G69" s="87"/>
-      <c r="H69" s="87"/>
-      <c r="I69" s="88"/>
-      <c r="J69" s="89"/>
-      <c r="K69" s="93"/>
+      <c r="E69" s="76"/>
+      <c r="F69" s="74"/>
+      <c r="G69" s="74"/>
+      <c r="H69" s="74"/>
+      <c r="I69" s="75"/>
+      <c r="J69" s="76"/>
+      <c r="K69" s="80"/>
     </row>
     <row r="70" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="96"/>
-      <c r="B70" s="87"/>
-      <c r="C70" s="88"/>
+      <c r="A70" s="99"/>
+      <c r="B70" s="74"/>
+      <c r="C70" s="75"/>
       <c r="D70" s="48"/>
-      <c r="E70" s="89"/>
-      <c r="F70" s="87"/>
-      <c r="G70" s="87"/>
-      <c r="H70" s="87"/>
-      <c r="I70" s="88"/>
-      <c r="J70" s="89"/>
-      <c r="K70" s="93"/>
+      <c r="E70" s="76"/>
+      <c r="F70" s="74"/>
+      <c r="G70" s="74"/>
+      <c r="H70" s="74"/>
+      <c r="I70" s="75"/>
+      <c r="J70" s="76"/>
+      <c r="K70" s="80"/>
     </row>
     <row r="71" spans="1:11" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="97"/>
-      <c r="B71" s="91"/>
-      <c r="C71" s="92"/>
+      <c r="A71" s="100"/>
+      <c r="B71" s="78"/>
+      <c r="C71" s="79"/>
       <c r="D71" s="49"/>
-      <c r="E71" s="90"/>
-      <c r="F71" s="91"/>
-      <c r="G71" s="91"/>
-      <c r="H71" s="91"/>
-      <c r="I71" s="92"/>
-      <c r="J71" s="90"/>
-      <c r="K71" s="94"/>
+      <c r="E71" s="77"/>
+      <c r="F71" s="78"/>
+      <c r="G71" s="78"/>
+      <c r="H71" s="78"/>
+      <c r="I71" s="79"/>
+      <c r="J71" s="77"/>
+      <c r="K71" s="81"/>
     </row>
     <row r="72" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="28" t="s">
@@ -10396,12 +10396,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:K6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A64:C71"/>
-    <mergeCell ref="E64:I71"/>
-    <mergeCell ref="J64:K71"/>
     <mergeCell ref="C5:K5"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A4:B4"/>
@@ -10413,6 +10407,12 @@
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:I3"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:K6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A64:C71"/>
+    <mergeCell ref="E64:I71"/>
+    <mergeCell ref="J64:K71"/>
   </mergeCells>
   <conditionalFormatting sqref="I49:I63">
     <cfRule type="cellIs" dxfId="79" priority="117" operator="equal">

</xml_diff>